<commit_message>
added check rank results
</commit_message>
<xml_diff>
--- a/test/snATAC_check_list_res_padj.xlsx
+++ b/test/snATAC_check_list_res_padj.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangcheng/github/atacMotif/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/github/atacMotif/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C29963-DC84-8049-9214-471270C95F40}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28280" yWindow="1040" windowWidth="34400" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="-40960" yWindow="460" windowWidth="40960" windowHeight="22580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="snATAC_check_list_res_padj" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="218">
   <si>
     <t>TF</t>
   </si>
@@ -47,9 +48,6 @@
     <t>genus.id</t>
   </si>
   <si>
-    <t>genus.name</t>
-  </si>
-  <si>
     <t>tf.symbol</t>
   </si>
   <si>
@@ -648,16 +646,67 @@
   </si>
   <si>
     <t>ENSG00000164985</t>
+  </si>
+  <si>
+    <t>MA0117.2</t>
+  </si>
+  <si>
+    <t>Mafb</t>
+  </si>
+  <si>
+    <t>Arx</t>
+  </si>
+  <si>
+    <t>MA0874.1</t>
+  </si>
+  <si>
+    <t>MA0631.1</t>
+  </si>
+  <si>
+    <t>Six3</t>
+  </si>
+  <si>
+    <t>ENSG00000129514</t>
+  </si>
+  <si>
+    <t>MA0078.1</t>
+  </si>
+  <si>
+    <t>Sox17</t>
+  </si>
+  <si>
+    <t>4.1.1.6.2</t>
+  </si>
+  <si>
+    <t>SOX17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.1.1.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -689,9 +738,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,8 +754,199 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>706966</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="plot" descr="/var/folders/sk/3l94pbjd1xdcdppx2x6tyq700000gn/T/com.microsoft.Excel/WebArchiveCopyPasteTempFiles/plot_zoom_png?width=622&amp;height=444">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{511887B3-A674-4F43-881C-C91DFE97FA0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="5410200"/>
+          <a:ext cx="5113866" cy="3835400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>61726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="plot" descr="/var/folders/sk/3l94pbjd1xdcdppx2x6tyq700000gn/T/com.microsoft.Excel/WebArchiveCopyPasteTempFiles/plot_zoom_png?width=422&amp;height=233">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12273118-E5C5-124F-B058-4D6D2F71C361}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5448300" y="5562599"/>
+          <a:ext cx="3733800" cy="2220727"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="plot" descr="/var/folders/sk/3l94pbjd1xdcdppx2x6tyq700000gn/T/com.microsoft.Excel/WebArchiveCopyPasteTempFiles/plot_zoom_png?width=736&amp;height=569">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C277692-7C5F-DC43-B584-8E0CC9A223ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9613900" y="5473699"/>
+          <a:ext cx="6362700" cy="4772025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -968,179 +1211,184 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" customWidth="1"/>
+    <col min="8" max="14" width="10.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1"/>
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+    </row>
+    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V2" t="s">
-        <v>29</v>
-      </c>
-      <c r="W2" t="s">
-        <v>29</v>
-      </c>
-      <c r="X2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>29</v>
+      <c r="O2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
@@ -1148,43 +1396,43 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>33</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>34</v>
-      </c>
-      <c r="N3" t="s">
-        <v>35</v>
       </c>
       <c r="O3" s="1">
         <v>68.36</v>
@@ -1199,114 +1447,114 @@
         <v>30.56</v>
       </c>
       <c r="S3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z3">
         <v>2.91</v>
       </c>
       <c r="AA3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="N4" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s">
-        <v>29</v>
-      </c>
-      <c r="S4" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" t="s">
-        <v>29</v>
-      </c>
-      <c r="W4" t="s">
-        <v>29</v>
-      </c>
-      <c r="X4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>29</v>
+      <c r="O4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -1314,49 +1562,49 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
         <v>50</v>
       </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
         <v>52</v>
       </c>
-      <c r="F5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" t="s">
         <v>53</v>
       </c>
-      <c r="H5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>54</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>55</v>
       </c>
-      <c r="L5" t="s">
-        <v>56</v>
-      </c>
       <c r="M5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" t="s">
         <v>48</v>
-      </c>
-      <c r="N5" t="s">
-        <v>49</v>
       </c>
       <c r="O5">
         <v>79.44</v>
       </c>
       <c r="P5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="1">
         <v>155.93</v>
@@ -1368,25 +1616,25 @@
         <v>42.69</v>
       </c>
       <c r="T5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X5">
         <v>2.52</v>
       </c>
       <c r="Y5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA5">
         <v>9.59</v>
@@ -1397,43 +1645,43 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" t="s">
         <v>60</v>
       </c>
-      <c r="H6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>61</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>62</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>63</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>64</v>
-      </c>
-      <c r="N6" t="s">
-        <v>65</v>
       </c>
       <c r="O6">
         <v>3.71</v>
@@ -1454,25 +1702,25 @@
         <v>30.75</v>
       </c>
       <c r="U6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X6">
         <v>5.59</v>
       </c>
       <c r="Y6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
@@ -1480,46 +1728,46 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>67</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>68</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" t="s">
         <v>69</v>
       </c>
-      <c r="F7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" t="s">
         <v>70</v>
       </c>
-      <c r="H7" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>71</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>72</v>
       </c>
-      <c r="L7" t="s">
-        <v>73</v>
-      </c>
       <c r="M7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" t="s">
         <v>64</v>
       </c>
-      <c r="N7" t="s">
-        <v>65</v>
-      </c>
       <c r="O7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P7">
         <v>12.92</v>
@@ -1537,25 +1785,25 @@
         <v>19.329999999999998</v>
       </c>
       <c r="U7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X7">
         <v>4.92</v>
       </c>
       <c r="Y7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
@@ -1563,43 +1811,43 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>75</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>76</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" t="s">
         <v>77</v>
       </c>
-      <c r="F8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>78</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" t="s">
         <v>79</v>
       </c>
-      <c r="I8" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>80</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>81</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>82</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>83</v>
-      </c>
-      <c r="N8" t="s">
-        <v>84</v>
       </c>
       <c r="O8">
         <v>29.76</v>
@@ -1620,7 +1868,7 @@
         <v>29.1</v>
       </c>
       <c r="U8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V8">
         <v>5.12</v>
@@ -1632,96 +1880,96 @@
         <v>5.24</v>
       </c>
       <c r="Y8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z8">
         <v>2.74</v>
       </c>
       <c r="AA8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="H9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="K9" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N9" t="s">
-        <v>92</v>
-      </c>
-      <c r="O9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S9" t="s">
-        <v>29</v>
-      </c>
-      <c r="T9" t="s">
-        <v>29</v>
-      </c>
-      <c r="U9" t="s">
-        <v>29</v>
-      </c>
-      <c r="V9" t="s">
-        <v>29</v>
-      </c>
-      <c r="W9" t="s">
-        <v>29</v>
-      </c>
-      <c r="X9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>29</v>
+      <c r="O9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
@@ -1729,82 +1977,82 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
         <v>93</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>94</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>95</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" t="s">
         <v>96</v>
       </c>
-      <c r="F10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" t="s">
         <v>97</v>
       </c>
-      <c r="H10" t="s">
-        <v>93</v>
-      </c>
-      <c r="I10" t="s">
-        <v>93</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>98</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>99</v>
       </c>
-      <c r="L10" t="s">
-        <v>100</v>
-      </c>
       <c r="M10" t="s">
+        <v>90</v>
+      </c>
+      <c r="N10" t="s">
         <v>91</v>
-      </c>
-      <c r="N10" t="s">
-        <v>92</v>
       </c>
       <c r="O10">
         <v>2.8</v>
       </c>
       <c r="P10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q10">
         <v>2.95</v>
       </c>
       <c r="R10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="V10" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="W10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
@@ -1812,43 +2060,43 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
         <v>101</v>
       </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>102</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" t="s">
         <v>103</v>
       </c>
-      <c r="F11" t="s">
-        <v>101</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>104</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" t="s">
         <v>105</v>
       </c>
-      <c r="I11" t="s">
-        <v>101</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>106</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>107</v>
       </c>
-      <c r="L11" t="s">
-        <v>108</v>
-      </c>
       <c r="M11" t="s">
+        <v>90</v>
+      </c>
+      <c r="N11" t="s">
         <v>91</v>
-      </c>
-      <c r="N11" t="s">
-        <v>92</v>
       </c>
       <c r="O11">
         <v>7.18</v>
@@ -1869,108 +2117,108 @@
         <v>22.62</v>
       </c>
       <c r="U11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X11">
         <v>6.06</v>
       </c>
       <c r="Y11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="H12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H12" t="s">
-        <v>109</v>
-      </c>
-      <c r="I12" t="s">
-        <v>109</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="K12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="K12" t="s">
-        <v>109</v>
-      </c>
-      <c r="L12" t="s">
-        <v>113</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="M12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="N12" t="s">
-        <v>92</v>
-      </c>
-      <c r="O12" t="s">
-        <v>29</v>
-      </c>
-      <c r="P12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>29</v>
-      </c>
-      <c r="R12" t="s">
-        <v>29</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U12" t="s">
-        <v>29</v>
-      </c>
-      <c r="V12" t="s">
-        <v>29</v>
-      </c>
-      <c r="W12" t="s">
-        <v>29</v>
-      </c>
-      <c r="X12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>29</v>
+      <c r="O12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
@@ -1978,49 +2226,49 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" t="s">
         <v>114</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>115</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>209</v>
+      </c>
+      <c r="F13" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" t="s">
         <v>116</v>
       </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" t="s">
+        <v>113</v>
+      </c>
+      <c r="J13" t="s">
         <v>117</v>
       </c>
-      <c r="H13" t="s">
-        <v>114</v>
-      </c>
-      <c r="I13" t="s">
-        <v>114</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
+        <v>113</v>
+      </c>
+      <c r="L13" t="s">
         <v>118</v>
       </c>
-      <c r="K13" t="s">
-        <v>114</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>119</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>120</v>
       </c>
-      <c r="N13" t="s">
-        <v>121</v>
-      </c>
       <c r="O13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q13">
         <v>1.82</v>
@@ -2032,28 +2280,28 @@
         <v>5.8</v>
       </c>
       <c r="T13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
@@ -2061,43 +2309,43 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s">
         <v>122</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>123</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
         <v>124</v>
       </c>
-      <c r="E14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" t="s">
         <v>125</v>
       </c>
-      <c r="H14" t="s">
-        <v>122</v>
-      </c>
-      <c r="I14" t="s">
-        <v>122</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>126</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>127</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>128</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>129</v>
-      </c>
-      <c r="N14" t="s">
-        <v>130</v>
       </c>
       <c r="O14" s="1">
         <v>1.95</v>
@@ -2106,120 +2354,120 @@
         <v>11.06</v>
       </c>
       <c r="Q14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R14">
         <v>14.27</v>
       </c>
       <c r="S14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="H15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H15" t="s">
-        <v>131</v>
-      </c>
-      <c r="I15" t="s">
-        <v>131</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="K15" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="N15" t="s">
-        <v>139</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U15" t="s">
-        <v>29</v>
-      </c>
-      <c r="V15" t="s">
-        <v>29</v>
-      </c>
-      <c r="W15" t="s">
-        <v>29</v>
-      </c>
-      <c r="X15" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>29</v>
+      <c r="O15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
@@ -2227,49 +2475,49 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
         <v>140</v>
       </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>141</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>139</v>
+      </c>
+      <c r="G16" t="s">
         <v>142</v>
       </c>
-      <c r="F16" t="s">
-        <v>140</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
+        <v>139</v>
+      </c>
+      <c r="I16" t="s">
+        <v>139</v>
+      </c>
+      <c r="J16" t="s">
         <v>143</v>
       </c>
-      <c r="H16" t="s">
-        <v>140</v>
-      </c>
-      <c r="I16" t="s">
-        <v>140</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>144</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>145</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>146</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>147</v>
-      </c>
-      <c r="N16" t="s">
-        <v>148</v>
       </c>
       <c r="O16">
         <v>6.93</v>
       </c>
       <c r="P16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q16" s="1">
         <v>4.4000000000000004</v>
@@ -2278,31 +2526,31 @@
         <v>9.1300000000000008</v>
       </c>
       <c r="S16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
@@ -2310,82 +2558,82 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
         <v>149</v>
       </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17" t="s">
+        <v>211</v>
+      </c>
+      <c r="G17" t="s">
         <v>150</v>
       </c>
-      <c r="E17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
+        <v>148</v>
+      </c>
+      <c r="I17" t="s">
+        <v>148</v>
+      </c>
+      <c r="J17" t="s">
         <v>151</v>
       </c>
-      <c r="H17" t="s">
-        <v>149</v>
-      </c>
-      <c r="I17" t="s">
-        <v>149</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>152</v>
       </c>
-      <c r="K17" t="s">
-        <v>153</v>
-      </c>
       <c r="L17" t="s">
+        <v>145</v>
+      </c>
+      <c r="M17" t="s">
         <v>146</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>147</v>
       </c>
-      <c r="N17" t="s">
-        <v>148</v>
-      </c>
       <c r="O17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AA17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
@@ -2393,165 +2641,165 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" t="s">
         <v>154</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>155</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>156</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>157</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>158</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
+        <v>153</v>
+      </c>
+      <c r="I18" t="s">
+        <v>153</v>
+      </c>
+      <c r="J18" t="s">
         <v>159</v>
       </c>
-      <c r="H18" t="s">
-        <v>154</v>
-      </c>
-      <c r="I18" t="s">
-        <v>154</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>160</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>161</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>162</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>163</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U18" t="s">
+        <v>28</v>
+      </c>
+      <c r="V18" t="s">
+        <v>28</v>
+      </c>
+      <c r="W18" t="s">
+        <v>28</v>
+      </c>
+      <c r="X18" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="O18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U18" t="s">
-        <v>29</v>
-      </c>
-      <c r="V18" t="s">
-        <v>29</v>
-      </c>
-      <c r="W18" t="s">
-        <v>29</v>
-      </c>
-      <c r="X18" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="H19" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="H19" t="s">
-        <v>165</v>
-      </c>
-      <c r="I19" t="s">
-        <v>165</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="K19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K19" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" t="s">
-        <v>29</v>
-      </c>
-      <c r="M19" t="s">
+      <c r="N19" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="N19" t="s">
-        <v>170</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S19" t="s">
-        <v>29</v>
-      </c>
-      <c r="T19" t="s">
-        <v>29</v>
-      </c>
-      <c r="U19" t="s">
-        <v>29</v>
-      </c>
-      <c r="V19" t="s">
-        <v>29</v>
-      </c>
-      <c r="W19" t="s">
-        <v>29</v>
-      </c>
-      <c r="X19" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>29</v>
+      <c r="O19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
@@ -2559,43 +2807,43 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" t="s">
         <v>171</v>
       </c>
-      <c r="C20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>172</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>170</v>
+      </c>
+      <c r="G20" t="s">
         <v>173</v>
       </c>
-      <c r="F20" t="s">
-        <v>171</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>174</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>175</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>176</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>177</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>178</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>179</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>180</v>
-      </c>
-      <c r="N20" t="s">
-        <v>181</v>
       </c>
       <c r="O20">
         <v>10.17</v>
@@ -2607,16 +2855,16 @@
         <v>7.27</v>
       </c>
       <c r="R20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S20">
         <v>36.74</v>
       </c>
       <c r="T20" t="s">
-        <v>29</v>
-      </c>
-      <c r="U20" t="s">
-        <v>182</v>
+        <v>28</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="V20" s="1">
         <v>67.099999999999994</v>
@@ -2642,70 +2890,70 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" t="s">
         <v>183</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>184</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>185</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" t="s">
         <v>186</v>
       </c>
-      <c r="F21" t="s">
-        <v>183</v>
-      </c>
-      <c r="G21" t="s">
-        <v>187</v>
-      </c>
       <c r="H21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J21" t="s">
+        <v>176</v>
+      </c>
+      <c r="K21" t="s">
         <v>177</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>178</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>179</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>180</v>
       </c>
-      <c r="N21" t="s">
-        <v>181</v>
-      </c>
       <c r="O21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S21" s="1">
         <v>11.4</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="V21">
         <v>49.95</v>
       </c>
       <c r="W21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X21" s="1">
         <v>15.64</v>
@@ -2725,61 +2973,61 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" t="s">
         <v>188</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>189</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>190</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
+        <v>187</v>
+      </c>
+      <c r="G22" t="s">
         <v>191</v>
       </c>
-      <c r="F22" t="s">
-        <v>188</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
+        <v>187</v>
+      </c>
+      <c r="I22" t="s">
+        <v>187</v>
+      </c>
+      <c r="J22" t="s">
         <v>192</v>
       </c>
-      <c r="H22" t="s">
-        <v>188</v>
-      </c>
-      <c r="I22" t="s">
-        <v>188</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>193</v>
       </c>
-      <c r="K22" t="s">
-        <v>194</v>
-      </c>
       <c r="L22" t="s">
+        <v>178</v>
+      </c>
+      <c r="M22" t="s">
         <v>179</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>180</v>
       </c>
-      <c r="N22" t="s">
-        <v>181</v>
-      </c>
       <c r="O22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S22" s="1">
         <v>9.6999999999999993</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U22">
         <v>320.29000000000002</v>
@@ -2788,7 +3036,7 @@
         <v>37.96</v>
       </c>
       <c r="W22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X22" s="1">
         <v>11.89</v>
@@ -2808,251 +3056,330 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" t="s">
         <v>195</v>
       </c>
-      <c r="C23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" t="s">
         <v>196</v>
       </c>
-      <c r="E23" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
+        <v>194</v>
+      </c>
+      <c r="I23" t="s">
+        <v>194</v>
+      </c>
+      <c r="J23" t="s">
         <v>197</v>
       </c>
-      <c r="H23" t="s">
-        <v>195</v>
-      </c>
-      <c r="I23" t="s">
-        <v>195</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>198</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>199</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>200</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>201</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
+        <v>28</v>
+      </c>
+      <c r="P23" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>28</v>
+      </c>
+      <c r="R23" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23" t="s">
+        <v>28</v>
+      </c>
+      <c r="T23" t="s">
+        <v>28</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W23" t="s">
+        <v>28</v>
+      </c>
+      <c r="X23" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="O23" t="s">
-        <v>29</v>
-      </c>
-      <c r="P23" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>29</v>
-      </c>
-      <c r="R23" t="s">
-        <v>29</v>
-      </c>
-      <c r="S23" t="s">
-        <v>29</v>
-      </c>
-      <c r="T23" t="s">
-        <v>29</v>
-      </c>
-      <c r="U23" t="s">
-        <v>29</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="W23" t="s">
-        <v>29</v>
-      </c>
-      <c r="X23" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>29</v>
+      <c r="C24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA24" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>203</v>
-      </c>
-      <c r="C24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" t="s">
+    <row r="25" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G24" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" t="s">
-        <v>29</v>
-      </c>
-      <c r="J24" t="s">
-        <v>29</v>
-      </c>
-      <c r="K24" t="s">
-        <v>29</v>
-      </c>
-      <c r="L24" t="s">
-        <v>29</v>
-      </c>
-      <c r="M24" t="s">
-        <v>29</v>
-      </c>
-      <c r="N24" t="s">
-        <v>29</v>
-      </c>
-      <c r="O24" t="s">
-        <v>29</v>
-      </c>
-      <c r="P24" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>29</v>
-      </c>
-      <c r="R24" t="s">
-        <v>29</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U24" t="s">
-        <v>29</v>
-      </c>
-      <c r="V24" t="s">
-        <v>29</v>
-      </c>
-      <c r="W24" t="s">
-        <v>29</v>
-      </c>
-      <c r="X24" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>29</v>
+      <c r="C25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA25" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>205</v>
-      </c>
-      <c r="C25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" t="s">
-        <v>206</v>
-      </c>
-      <c r="E25" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" t="s">
-        <v>29</v>
-      </c>
-      <c r="I25" t="s">
-        <v>29</v>
-      </c>
-      <c r="J25" t="s">
-        <v>29</v>
-      </c>
-      <c r="K25" t="s">
-        <v>29</v>
-      </c>
-      <c r="L25" t="s">
-        <v>29</v>
-      </c>
-      <c r="M25" t="s">
-        <v>29</v>
-      </c>
-      <c r="N25" t="s">
-        <v>29</v>
-      </c>
-      <c r="O25" t="s">
-        <v>29</v>
-      </c>
-      <c r="P25" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>29</v>
-      </c>
-      <c r="R25" t="s">
-        <v>29</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U25" t="s">
-        <v>29</v>
-      </c>
-      <c r="V25" t="s">
-        <v>29</v>
-      </c>
-      <c r="W25" t="s">
-        <v>29</v>
-      </c>
-      <c r="X25" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>29</v>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>216</v>
+      </c>
+      <c r="D26" t="s">
+        <v>212</v>
+      </c>
+      <c r="E26" t="s">
+        <v>213</v>
+      </c>
+      <c r="F26" t="s">
+        <v>214</v>
+      </c>
+      <c r="G26" t="s">
+        <v>215</v>
+      </c>
+      <c r="H26" t="s">
+        <v>216</v>
+      </c>
+      <c r="I26" t="s">
+        <v>216</v>
+      </c>
+      <c r="J26" t="s">
+        <v>217</v>
+      </c>
+      <c r="K26" t="s">
+        <v>198</v>
+      </c>
+      <c r="L26" t="s">
+        <v>199</v>
+      </c>
+      <c r="M26" t="s">
+        <v>200</v>
+      </c>
+      <c r="N26" t="s">
+        <v>201</v>
+      </c>
+      <c r="O26" t="s">
+        <v>28</v>
+      </c>
+      <c r="P26" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>28</v>
+      </c>
+      <c r="R26" t="s">
+        <v>28</v>
+      </c>
+      <c r="S26" t="s">
+        <v>28</v>
+      </c>
+      <c r="T26" t="s">
+        <v>28</v>
+      </c>
+      <c r="U26" s="1">
+        <v>12.3</v>
+      </c>
+      <c r="V26" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="W26" t="s">
+        <v>28</v>
+      </c>
+      <c r="X26" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="52" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added test into ignore
</commit_message>
<xml_diff>
--- a/test/snATAC_check_list_res_padj.xlsx
+++ b/test/snATAC_check_list_res_padj.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/github/atacMotif/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C29963-DC84-8049-9214-471270C95F40}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844CF23F-541F-1347-B850-10EEA00C2CF2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40960" yWindow="460" windowWidth="40960" windowHeight="22580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="snATAC_check_list_res_padj" sheetId="1" r:id="rId1"/>
@@ -772,9 +772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>706966</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -805,7 +805,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="5410200"/>
-          <a:ext cx="5113866" cy="3835400"/>
+          <a:ext cx="4673599" cy="3505200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -826,16 +826,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>12699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>61726</xdr:rowOff>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>201426</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -865,7 +865,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5448300" y="5562599"/>
+          <a:off x="5003800" y="5499099"/>
           <a:ext cx="3733800" cy="2220727"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -887,16 +887,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>63499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>53974</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -926,8 +926,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9613900" y="5473699"/>
-          <a:ext cx="6362700" cy="4772025"/>
+          <a:off x="9156700" y="5346699"/>
+          <a:ext cx="5676900" cy="4257675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1217,8 +1217,8 @@
   </sheetPr>
   <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AD24" sqref="AD24"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>